<commit_message>
Added Test cases for Logout Functionality
</commit_message>
<xml_diff>
--- a/world remit test scenarios 1.xlsx
+++ b/world remit test scenarios 1.xlsx
@@ -8,46 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\archa\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9F95A5EB-6187-48D3-BD92-9C5EBDDEBF45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B237E732-47CE-4218-9033-42E86BA4AD46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test scenarios" sheetId="1" r:id="rId1"/>
     <sheet name="Sign up" sheetId="2" r:id="rId2"/>
     <sheet name="Log In" sheetId="3" r:id="rId3"/>
+    <sheet name="Logout" sheetId="4" r:id="rId4"/>
+    <sheet name="Home page" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
-    <externalReference r:id="rId5"/>
-    <externalReference r:id="rId6"/>
     <externalReference r:id="rId7"/>
-    <externalReference r:id="rId8"/>
-    <externalReference r:id="rId9"/>
-    <externalReference r:id="rId10"/>
-    <externalReference r:id="rId11"/>
-    <externalReference r:id="rId12"/>
-    <externalReference r:id="rId13"/>
-    <externalReference r:id="rId14"/>
-    <externalReference r:id="rId15"/>
-    <externalReference r:id="rId16"/>
-    <externalReference r:id="rId17"/>
-    <externalReference r:id="rId18"/>
-    <externalReference r:id="rId19"/>
-    <externalReference r:id="rId20"/>
-    <externalReference r:id="rId21"/>
-    <externalReference r:id="rId22"/>
-    <externalReference r:id="rId23"/>
-    <externalReference r:id="rId24"/>
-    <externalReference r:id="rId25"/>
-    <externalReference r:id="rId26"/>
-    <externalReference r:id="rId27"/>
-    <externalReference r:id="rId28"/>
-    <externalReference r:id="rId29"/>
-    <externalReference r:id="rId30"/>
-    <externalReference r:id="rId31"/>
-    <externalReference r:id="rId32"/>
-    <externalReference r:id="rId33"/>
   </externalReferences>
   <calcPr calcId="191028"/>
   <extLst>
@@ -70,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="238">
   <si>
     <t>Test Scenario ID</t>
   </si>
@@ -97,6 +71,13 @@
   </si>
   <si>
     <t>Validate the working of Logout functionality</t>
+  </si>
+  <si>
+    <t>(TS_004)
+Home page Functionaly</t>
+  </si>
+  <si>
+    <t>Validate the working of Home page functionality</t>
   </si>
   <si>
     <t>Test Case ID</t>
@@ -883,12 +864,175 @@
   <si>
     <t>1. Login page should be attrective and easy to understand.</t>
   </si>
+  <si>
+    <t>TC_LOF_001</t>
+  </si>
+  <si>
+    <t>Verify logging out by selecting Logout function.</t>
+  </si>
+  <si>
+    <t>1. Open the Application URL (https://www.worldremit.com) 
+2. User should be logged in.</t>
+  </si>
+  <si>
+    <t>1. Select 'my account' drop menu 
+2. click on 'LOGOUT' option (ER-1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. User should be log out and directly navigating to the 'LOG IN' page. </t>
+  </si>
+  <si>
+    <t>TC_LOF_002</t>
+  </si>
+  <si>
+    <t>Verify logging out and browsing back</t>
+  </si>
+  <si>
+    <t>1. Select 'my account' drop menu 
+2. click on 'LOGOUT' option (ER-1)
+3. Click on Browser back button (ER-2)(AR-1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. User should be log out and directly navigating to the 'LOG IN' page. 
+2. User should not be logged in again </t>
+  </si>
+  <si>
+    <t>1. User is getting 'LOG IN' again</t>
+  </si>
+  <si>
+    <t>TC_LOF_003</t>
+  </si>
+  <si>
+    <t>Verify there is no logout option before login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Click on 'MY ACCOUNT' drop menu </t>
+  </si>
+  <si>
+    <t>1. Log out option should not be displayed before login.</t>
+  </si>
+  <si>
+    <t>TC_LOF_004</t>
+  </si>
+  <si>
+    <t>Verify logout from your account and check logout from every places where you logged in</t>
+  </si>
+  <si>
+    <t>1. Open the Application URL (https://www.worldremit.com) 
+2. Try to login in fire fox browser
+3. Again login in chrome browser in mobile device.</t>
+  </si>
+  <si>
+    <t>1. Try to 'LOGIN' in firefox browser in laptop and 'LOGIN' in chrome browser in mobile device.
+1. Click on 'MY ACCOUNT' drop menu from fire fox browser.
+2. Click on 'LOG OUT' function from firefox browser (ER-1)(AR-1)</t>
+  </si>
+  <si>
+    <t>1. User should be logged out from both browser and both devices.</t>
+  </si>
+  <si>
+    <t>1. User is not 'LOGGING OUT' from chrome browser in mobile device.</t>
+  </si>
+  <si>
+    <t>TC_LOF_005</t>
+  </si>
+  <si>
+    <t>Verify LOGOUT button container</t>
+  </si>
+  <si>
+    <t>1. Select 'my account' drop menu 
+2. Move curser to 'LOGOUT' button container (ER-1)
+3. Try to click on high lighted container (where LOGOUT words are not popped up)(ER-2)(AR-1)(AR-2)</t>
+  </si>
+  <si>
+    <t>1. The whole LOGOUT button container should be high lighted.
+2. The high lighted container of LOGOUT button should be clickable.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. the whole LOGOUT button container is not clickable. 
+2. User are able to LOGOUT when user is clicking only LOGOUT word. </t>
+  </si>
+  <si>
+    <t>TC_LOF_006</t>
+  </si>
+  <si>
+    <t>Verify whole LOGOUT page</t>
+  </si>
+  <si>
+    <t>1. Select 'my account' drop menu 
+2. click on 'LOGOUT' option (ER-1)
+3. Check all links of logout page (ER-2)</t>
+  </si>
+  <si>
+    <t>1. User should be log out. 
+2. All links should be working properly and by selecting it should be navigating with respectively.</t>
+  </si>
+  <si>
+    <t>TC_LOF_007</t>
+  </si>
+  <si>
+    <t>Verify the navigating page after LOGOUT</t>
+  </si>
+  <si>
+    <t>1. It is directly navigating to LOGIN page.</t>
+  </si>
+  <si>
+    <t>1. User should not able to see home page as it is navigating to LOGIN page only.</t>
+  </si>
+  <si>
+    <t>TC_HP_001</t>
+  </si>
+  <si>
+    <t>TS_004
+Home page Functionaly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify main functionality of currency exchange rate </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Check the exchange rate title are there with currency
+2. whenever you change the currency the title shoul;d be change
+ </t>
+  </si>
+  <si>
+    <t>TC_HP_002</t>
+  </si>
+  <si>
+    <t>TC_HP_003</t>
+  </si>
+  <si>
+    <t>TC_HP_004</t>
+  </si>
+  <si>
+    <t>TC_HP_005</t>
+  </si>
+  <si>
+    <t>TC_HP_006</t>
+  </si>
+  <si>
+    <t>TC_HP_007</t>
+  </si>
+  <si>
+    <t>TC_HP_008</t>
+  </si>
+  <si>
+    <t>TC_HP_009</t>
+  </si>
+  <si>
+    <t>TC_HP_010</t>
+  </si>
+  <si>
+    <t>TC_HP_011</t>
+  </si>
+  <si>
+    <t>TC_HP_012</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1015,6 +1159,15 @@
       <sz val="12"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1041,7 +1194,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1156,12 +1309,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1233,9 +1399,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1339,42 +1502,298 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <sz val="12"/>
+        <name val="Arial"/>
+      </font>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <sz val="12"/>
+        <name val="Arial"/>
+      </font>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <sz val="12"/>
+        <name val="Arial"/>
+      </font>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <sz val="12"/>
+        <name val="Arial"/>
+      </font>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <sz val="12"/>
+        <name val="Arial"/>
+      </font>
+      <alignment wrapText="1"/>
+      <border>
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1391,305 +1810,6 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Logout"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink10.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Checkout"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink11.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="My Account"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink12.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="My Account Information"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink13.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Change Password"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink14.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Address Book"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink15.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Order History"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink16.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Order Information"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink17.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Product Returns"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink18.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Downloads"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink19.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Reward Points"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Forgot Password"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink20.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Returns"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink21.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Transactions"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink22.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Recurring Payments"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink23.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Affiliate"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink24.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Newsletter"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink25.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Contact Us"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink26.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Gift Certificate"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink27.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Specail Offers"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink28.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Header Menu Footer Options"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink29.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Currencies"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Search"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink30.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
       <sheetName val="Register"/>
     </sheetNames>
     <sheetDataSet>
@@ -1699,82 +1819,27 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Product Compare"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Product Display Page"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink6.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Add to Cart"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink7.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Wish List"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink8.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Shopping Cart"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink9.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Home Page"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{03644E9F-9DE4-46AE-883A-403D9906BBC2}" name="Table1" displayName="Table1" ref="A3:E33" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" headerRowBorderDxfId="6" tableBorderDxfId="7" totalsRowBorderDxfId="5">
+  <autoFilter ref="A3:E33" xr:uid="{03644E9F-9DE4-46AE-883A-403D9906BBC2}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:B33">
+    <sortCondition ref="A3:A33"/>
+  </sortState>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{60C7A49C-1F75-4353-A4CB-5FE929816BEE}" name="TC_HP_001" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{CC2F7BA3-F5C9-46D4-A67F-590D7FC8AAC5}" name="TS_004_x000a_Home page Functionaly" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{BD724221-D339-4580-BF2D-05906248CD20}" name="Verify main functionality of currency exchange rate " dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{35FF8C30-B29E-4902-AC23-52F347841A99}" name="1. Open the Application URL (https://www.worldremit.com) _x000a_" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{CBDE764E-182B-46AB-9E3F-6BF89AA7A93B}" name="1. Check the exchange rate title are there with currency_x000a_2. whenever you change the currency the title shoul;d be change_x000a_ " dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2077,7 +2142,7 @@
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" customHeight="1"/>
@@ -2119,9 +2184,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="27"/>
-      <c r="B5" s="25"/>
+    <row r="5" spans="1:2" ht="30.75">
+      <c r="A5" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="27"/>
@@ -2236,6 +2305,7 @@
     <hyperlink ref="A2" location="'Sign up'!A1" display="(TS_001) _x000a_Sign Up Functionality" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="A3" location="'Log In'!A1" display="(TS_002) _x000a_Login Functionality" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="A4" location="Logout!A1" display="Logout!A1" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="A5" location="'Home page'!A1" display="(TS_004)_x000a_Home page Functionaly" xr:uid="{3925BDD1-8363-43D7-ABB4-0F5C7228CD7D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2245,18 +2315,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
+    <sheetView zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="15.140625" style="66" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" style="67" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.42578125" style="70" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" style="64" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" style="65" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.42578125" style="68" customWidth="1"/>
     <col min="4" max="4" width="23.85546875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="69.42578125" style="71" customWidth="1"/>
-    <col min="6" max="6" width="21.85546875" style="67" customWidth="1"/>
+    <col min="5" max="5" width="69.42578125" style="69" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" style="65" customWidth="1"/>
     <col min="7" max="7" width="55.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="54.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.42578125" style="3" bestFit="1" customWidth="1"/>
@@ -2265,736 +2335,736 @@
     <col min="12" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="74" customFormat="1" ht="15.75">
-      <c r="A1" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="44" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="44" t="s">
+    <row r="1" spans="1:11" s="72" customFormat="1" ht="15.75">
+      <c r="A1" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="44" t="s">
+      <c r="B1" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="44" t="s">
+      <c r="C1" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="44" t="s">
+      <c r="D1" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="44" t="s">
+      <c r="E1" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="44" t="s">
+      <c r="F1" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="44" t="s">
+      <c r="G1" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="44" t="s">
+      <c r="H1" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="44" t="s">
+      <c r="I1" s="43" t="s">
         <v>18</v>
       </c>
+      <c r="J1" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="43" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="15">
-      <c r="A2" s="65" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55"/>
+      <c r="A2" s="92" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="92"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
     </row>
     <row r="3" spans="1:11" ht="199.5">
-      <c r="A3" s="51" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="45" t="s">
+      <c r="A3" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="57" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="40" t="s">
+      <c r="C3" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="53" t="s">
+      <c r="D3" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="47" t="s">
+      <c r="E3" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="59"/>
-      <c r="I3" s="58"/>
-      <c r="J3" s="60"/>
-      <c r="K3" s="58"/>
+      <c r="F3" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="46" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="58"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="59"/>
+      <c r="K3" s="57"/>
     </row>
     <row r="4" spans="1:11" ht="189" customHeight="1">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="45" t="s">
+      <c r="G4" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="58"/>
+      <c r="I4" s="57"/>
+      <c r="J4" s="59"/>
+      <c r="K4" s="57"/>
+    </row>
+    <row r="5" spans="1:11" ht="153">
+      <c r="A5" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="40" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="57" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="40" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="53" t="s">
+      <c r="C5" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="47" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="59"/>
-      <c r="I4" s="58"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="58"/>
-    </row>
-    <row r="5" spans="1:11" ht="153">
-      <c r="A5" s="51" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="45" t="s">
+      <c r="E5" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" s="58"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="59"/>
+      <c r="K5" s="57"/>
+    </row>
+    <row r="6" spans="1:11" ht="168">
+      <c r="A6" s="50" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="40" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="57" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" s="53" t="s">
+      <c r="C6" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="47" t="s">
-        <v>33</v>
-      </c>
-      <c r="H5" s="59"/>
-      <c r="I5" s="58"/>
-      <c r="J5" s="60"/>
-      <c r="K5" s="58"/>
-    </row>
-    <row r="6" spans="1:11" ht="168">
-      <c r="A6" s="51" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" s="45" t="s">
+      <c r="E6" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="46" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" s="58"/>
+      <c r="I6" s="57"/>
+      <c r="J6" s="59"/>
+      <c r="K6" s="57"/>
+    </row>
+    <row r="7" spans="1:11" ht="122.25">
+      <c r="A7" s="50" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="40" t="s">
+      <c r="C7" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" s="60" t="s">
+        <v>44</v>
+      </c>
+      <c r="I7" s="57"/>
+      <c r="J7" s="59"/>
+      <c r="K7" s="57"/>
+    </row>
+    <row r="8" spans="1:11" ht="76.5">
+      <c r="A8" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="46" t="s">
+        <v>48</v>
+      </c>
+      <c r="H8" s="58"/>
+      <c r="I8" s="57"/>
+      <c r="J8" s="59"/>
+      <c r="K8" s="57"/>
+    </row>
+    <row r="9" spans="1:11" ht="91.5">
+      <c r="A9" s="50" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" s="51"/>
+      <c r="G9" s="46" t="s">
+        <v>52</v>
+      </c>
+      <c r="H9" s="58"/>
+      <c r="I9" s="57"/>
+      <c r="J9" s="59"/>
+      <c r="K9" s="57"/>
+    </row>
+    <row r="10" spans="1:11" ht="184.5">
+      <c r="A10" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" s="51"/>
+      <c r="G10" s="46" t="s">
+        <v>56</v>
+      </c>
+      <c r="H10" s="58"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="59"/>
+      <c r="K10" s="57"/>
+    </row>
+    <row r="11" spans="1:11" ht="153" customHeight="1">
+      <c r="A11" s="50" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="F11" s="51" t="s">
+        <v>60</v>
+      </c>
+      <c r="G11" s="46" t="s">
+        <v>61</v>
+      </c>
+      <c r="H11" s="58"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="59"/>
+      <c r="K11" s="57"/>
+    </row>
+    <row r="12" spans="1:11" ht="111" customHeight="1">
+      <c r="A12" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="F12" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="46" t="s">
+        <v>65</v>
+      </c>
+      <c r="H12" s="58"/>
+      <c r="I12" s="57"/>
+      <c r="J12" s="59"/>
+      <c r="K12" s="57"/>
+    </row>
+    <row r="13" spans="1:11" ht="108.75" customHeight="1">
+      <c r="A13" s="50" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="46" t="s">
+        <v>69</v>
+      </c>
+      <c r="H13" s="58"/>
+      <c r="I13" s="57"/>
+      <c r="J13" s="59"/>
+      <c r="K13" s="57"/>
+    </row>
+    <row r="14" spans="1:11" ht="101.25" customHeight="1">
+      <c r="A14" s="50" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" s="46" t="s">
+        <v>73</v>
+      </c>
+      <c r="H14" s="58"/>
+      <c r="I14" s="57"/>
+      <c r="J14" s="59"/>
+      <c r="K14" s="57"/>
+    </row>
+    <row r="15" spans="1:11" ht="104.25" customHeight="1">
+      <c r="A15" s="50" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="F15" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="H15" s="58"/>
+      <c r="I15" s="57"/>
+      <c r="J15" s="59"/>
+      <c r="K15" s="57"/>
+    </row>
+    <row r="16" spans="1:11" ht="90.75" customHeight="1">
+      <c r="A16" s="50" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="39" t="s">
+        <v>80</v>
+      </c>
+      <c r="F16" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="H16" s="58"/>
+      <c r="I16" s="57"/>
+      <c r="J16" s="59"/>
+      <c r="K16" s="57"/>
+    </row>
+    <row r="17" spans="1:11" ht="92.25" customHeight="1">
+      <c r="A17" s="50" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="39" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="F17" s="51" t="s">
+        <v>84</v>
+      </c>
+      <c r="G17" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="57" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="40" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" s="53" t="s">
+      <c r="H17" s="58"/>
+      <c r="I17" s="57"/>
+      <c r="J17" s="59"/>
+      <c r="K17" s="57"/>
+    </row>
+    <row r="18" spans="1:11" ht="129.75" customHeight="1">
+      <c r="A18" s="50" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="D18" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="47" t="s">
-        <v>37</v>
-      </c>
-      <c r="H6" s="59"/>
-      <c r="I6" s="58"/>
-      <c r="J6" s="60"/>
-      <c r="K6" s="58"/>
-    </row>
-    <row r="7" spans="1:11" ht="122.25">
-      <c r="A7" s="51" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7" s="45" t="s">
+      <c r="E18" s="39" t="s">
+        <v>87</v>
+      </c>
+      <c r="F18" s="52" t="s">
+        <v>88</v>
+      </c>
+      <c r="G18" s="46" t="s">
+        <v>89</v>
+      </c>
+      <c r="H18" s="58"/>
+      <c r="I18" s="57"/>
+      <c r="J18" s="59"/>
+      <c r="K18" s="57"/>
+    </row>
+    <row r="19" spans="1:11" ht="123" customHeight="1">
+      <c r="A19" s="50" t="s">
+        <v>90</v>
+      </c>
+      <c r="B19" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="40" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" s="57" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" s="53" t="s">
+      <c r="C19" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="D19" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="47" t="s">
-        <v>41</v>
-      </c>
-      <c r="H7" s="61" t="s">
-        <v>42</v>
-      </c>
-      <c r="I7" s="58"/>
-      <c r="J7" s="60"/>
-      <c r="K7" s="58"/>
-    </row>
-    <row r="8" spans="1:11" ht="76.5">
-      <c r="A8" s="51" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="45" t="s">
+      <c r="E19" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="F19" s="52" t="s">
+        <v>93</v>
+      </c>
+      <c r="G19" s="46" t="s">
+        <v>94</v>
+      </c>
+      <c r="H19" s="53" t="s">
+        <v>95</v>
+      </c>
+      <c r="I19" s="57"/>
+      <c r="J19" s="59"/>
+      <c r="K19" s="57"/>
+    </row>
+    <row r="20" spans="1:11" ht="102" customHeight="1">
+      <c r="A20" s="50" t="s">
+        <v>96</v>
+      </c>
+      <c r="B20" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="40" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" s="57" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="40" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" s="53" t="s">
+      <c r="C20" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="D20" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="47" t="s">
-        <v>46</v>
-      </c>
-      <c r="H8" s="59"/>
-      <c r="I8" s="58"/>
-      <c r="J8" s="60"/>
-      <c r="K8" s="58"/>
-    </row>
-    <row r="9" spans="1:11" ht="91.5">
-      <c r="A9" s="51" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" s="45" t="s">
+      <c r="E20" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="F20" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="G20" s="46" t="s">
+        <v>99</v>
+      </c>
+      <c r="H20" s="58"/>
+      <c r="I20" s="57"/>
+      <c r="J20" s="59"/>
+      <c r="K20" s="57"/>
+    </row>
+    <row r="21" spans="1:11" ht="78" customHeight="1">
+      <c r="A21" s="50" t="s">
+        <v>100</v>
+      </c>
+      <c r="B21" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="40" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" s="57" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="40" t="s">
-        <v>49</v>
-      </c>
-      <c r="F9" s="52"/>
-      <c r="G9" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="H9" s="59"/>
-      <c r="I9" s="58"/>
-      <c r="J9" s="60"/>
-      <c r="K9" s="58"/>
-    </row>
-    <row r="10" spans="1:11" ht="184.5">
-      <c r="A10" s="51" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" s="45" t="s">
+      <c r="C21" s="39" t="s">
+        <v>101</v>
+      </c>
+      <c r="D21" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="39" t="s">
+        <v>102</v>
+      </c>
+      <c r="F21" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="G21" s="46" t="s">
+        <v>103</v>
+      </c>
+      <c r="H21" s="58"/>
+      <c r="I21" s="57"/>
+      <c r="J21" s="59"/>
+      <c r="K21" s="57"/>
+    </row>
+    <row r="22" spans="1:11" ht="69" customHeight="1">
+      <c r="A22" s="50" t="s">
+        <v>104</v>
+      </c>
+      <c r="B22" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="40" t="s">
-        <v>52</v>
-      </c>
-      <c r="D10" s="57" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="40" t="s">
-        <v>53</v>
-      </c>
-      <c r="F10" s="52"/>
-      <c r="G10" s="47" t="s">
-        <v>54</v>
-      </c>
-      <c r="H10" s="59"/>
-      <c r="I10" s="58"/>
-      <c r="J10" s="60"/>
-      <c r="K10" s="58"/>
-    </row>
-    <row r="11" spans="1:11" ht="153" customHeight="1">
-      <c r="A11" s="51" t="s">
-        <v>55</v>
-      </c>
-      <c r="B11" s="45" t="s">
+      <c r="C22" s="39" t="s">
+        <v>105</v>
+      </c>
+      <c r="D22" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" s="39" t="s">
+        <v>106</v>
+      </c>
+      <c r="F22" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="G22" s="46" t="s">
+        <v>107</v>
+      </c>
+      <c r="H22" s="58"/>
+      <c r="I22" s="57"/>
+      <c r="J22" s="59"/>
+      <c r="K22" s="57"/>
+    </row>
+    <row r="23" spans="1:11" ht="124.5" customHeight="1">
+      <c r="A23" s="50" t="s">
+        <v>108</v>
+      </c>
+      <c r="B23" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="D11" s="57" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="F11" s="52" t="s">
-        <v>58</v>
-      </c>
-      <c r="G11" s="47" t="s">
-        <v>59</v>
-      </c>
-      <c r="H11" s="59"/>
-      <c r="I11" s="58"/>
-      <c r="J11" s="60"/>
-      <c r="K11" s="58"/>
-    </row>
-    <row r="12" spans="1:11" ht="111" customHeight="1">
-      <c r="A12" s="51" t="s">
-        <v>60</v>
-      </c>
-      <c r="B12" s="45" t="s">
+      <c r="C23" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="D23" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" s="39" t="s">
+        <v>110</v>
+      </c>
+      <c r="F23" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="G23" s="46" t="s">
+        <v>111</v>
+      </c>
+      <c r="H23" s="58"/>
+      <c r="I23" s="57"/>
+      <c r="J23" s="59"/>
+      <c r="K23" s="57"/>
+    </row>
+    <row r="24" spans="1:11" ht="107.25">
+      <c r="A24" s="50" t="s">
+        <v>112</v>
+      </c>
+      <c r="B24" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="40" t="s">
-        <v>61</v>
-      </c>
-      <c r="D12" s="57" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="F12" s="53" t="s">
+      <c r="C24" s="39" t="s">
+        <v>113</v>
+      </c>
+      <c r="D24" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="47" t="s">
-        <v>63</v>
-      </c>
-      <c r="H12" s="59"/>
-      <c r="I12" s="58"/>
-      <c r="J12" s="60"/>
-      <c r="K12" s="58"/>
-    </row>
-    <row r="13" spans="1:11" ht="108.75" customHeight="1">
-      <c r="A13" s="51" t="s">
-        <v>64</v>
-      </c>
-      <c r="B13" s="45" t="s">
+      <c r="E24" s="39" t="s">
+        <v>114</v>
+      </c>
+      <c r="F24" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="G24" s="46" t="s">
+        <v>115</v>
+      </c>
+      <c r="H24" s="58" t="s">
+        <v>116</v>
+      </c>
+      <c r="I24" s="57"/>
+      <c r="J24" s="59"/>
+      <c r="K24" s="57"/>
+    </row>
+    <row r="25" spans="1:11" ht="91.5">
+      <c r="A25" s="50" t="s">
+        <v>117</v>
+      </c>
+      <c r="B25" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="40" t="s">
-        <v>65</v>
-      </c>
-      <c r="D13" s="57" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="40" t="s">
-        <v>66</v>
-      </c>
-      <c r="F13" s="53" t="s">
+      <c r="C25" s="39" t="s">
+        <v>113</v>
+      </c>
+      <c r="D25" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="H13" s="59"/>
-      <c r="I13" s="58"/>
-      <c r="J13" s="60"/>
-      <c r="K13" s="58"/>
-    </row>
-    <row r="14" spans="1:11" ht="101.25" customHeight="1">
-      <c r="A14" s="51" t="s">
-        <v>68</v>
-      </c>
-      <c r="B14" s="45" t="s">
+      <c r="E25" s="39" t="s">
+        <v>118</v>
+      </c>
+      <c r="F25" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="G25" s="46" t="s">
+        <v>119</v>
+      </c>
+      <c r="H25" s="58"/>
+      <c r="I25" s="57"/>
+      <c r="J25" s="59"/>
+      <c r="K25" s="57"/>
+    </row>
+    <row r="26" spans="1:11" ht="74.25" customHeight="1">
+      <c r="A26" s="50" t="s">
+        <v>120</v>
+      </c>
+      <c r="B26" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="40" t="s">
-        <v>69</v>
-      </c>
-      <c r="D14" s="57" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" s="40" t="s">
-        <v>70</v>
-      </c>
-      <c r="F14" s="53" t="s">
+      <c r="C26" s="39" t="s">
+        <v>121</v>
+      </c>
+      <c r="D26" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="47" t="s">
-        <v>71</v>
-      </c>
-      <c r="H14" s="59"/>
-      <c r="I14" s="58"/>
-      <c r="J14" s="60"/>
-      <c r="K14" s="58"/>
-    </row>
-    <row r="15" spans="1:11" ht="104.25" customHeight="1">
-      <c r="A15" s="51" t="s">
-        <v>72</v>
-      </c>
-      <c r="B15" s="45" t="s">
+      <c r="E26" s="39" t="s">
+        <v>122</v>
+      </c>
+      <c r="F26" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="G26" s="46" t="s">
+        <v>123</v>
+      </c>
+      <c r="H26" s="58"/>
+      <c r="I26" s="57"/>
+      <c r="J26" s="59"/>
+      <c r="K26" s="57"/>
+    </row>
+    <row r="27" spans="1:11" s="6" customFormat="1" ht="83.25" customHeight="1">
+      <c r="A27" s="50" t="s">
+        <v>120</v>
+      </c>
+      <c r="B27" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="40" t="s">
-        <v>73</v>
-      </c>
-      <c r="D15" s="57" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="F15" s="53" t="s">
+      <c r="C27" s="67" t="s">
+        <v>124</v>
+      </c>
+      <c r="D27" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="G15" s="47" t="s">
-        <v>75</v>
-      </c>
-      <c r="H15" s="59"/>
-      <c r="I15" s="58"/>
-      <c r="J15" s="60"/>
-      <c r="K15" s="58"/>
-    </row>
-    <row r="16" spans="1:11" ht="90.75" customHeight="1">
-      <c r="A16" s="51" t="s">
-        <v>76</v>
-      </c>
-      <c r="B16" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" s="40" t="s">
-        <v>77</v>
-      </c>
-      <c r="D16" s="57" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" s="40" t="s">
-        <v>78</v>
-      </c>
-      <c r="F16" s="53" t="s">
-        <v>24</v>
-      </c>
-      <c r="G16" s="47" t="s">
-        <v>75</v>
-      </c>
-      <c r="H16" s="59"/>
-      <c r="I16" s="58"/>
-      <c r="J16" s="60"/>
-      <c r="K16" s="58"/>
-    </row>
-    <row r="17" spans="1:11" ht="92.25" customHeight="1">
-      <c r="A17" s="51" t="s">
-        <v>79</v>
-      </c>
-      <c r="B17" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="C17" s="40" t="s">
-        <v>80</v>
-      </c>
-      <c r="D17" s="57" t="s">
-        <v>22</v>
-      </c>
-      <c r="E17" s="40" t="s">
-        <v>81</v>
-      </c>
-      <c r="F17" s="52" t="s">
-        <v>82</v>
-      </c>
-      <c r="G17" s="47" t="s">
-        <v>33</v>
-      </c>
-      <c r="H17" s="59"/>
-      <c r="I17" s="58"/>
-      <c r="J17" s="60"/>
-      <c r="K17" s="58"/>
-    </row>
-    <row r="18" spans="1:11" ht="129.75" customHeight="1">
-      <c r="A18" s="51" t="s">
-        <v>83</v>
-      </c>
-      <c r="B18" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" s="40" t="s">
-        <v>84</v>
-      </c>
-      <c r="D18" s="57" t="s">
-        <v>22</v>
-      </c>
-      <c r="E18" s="40" t="s">
-        <v>85</v>
-      </c>
-      <c r="F18" s="53" t="s">
-        <v>86</v>
-      </c>
-      <c r="G18" s="47" t="s">
-        <v>87</v>
-      </c>
-      <c r="H18" s="59"/>
-      <c r="I18" s="58"/>
-      <c r="J18" s="60"/>
-      <c r="K18" s="58"/>
-    </row>
-    <row r="19" spans="1:11" ht="123" customHeight="1">
-      <c r="A19" s="51" t="s">
-        <v>88</v>
-      </c>
-      <c r="B19" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="C19" s="40" t="s">
-        <v>89</v>
-      </c>
-      <c r="D19" s="57" t="s">
-        <v>22</v>
-      </c>
-      <c r="E19" s="40" t="s">
-        <v>90</v>
-      </c>
-      <c r="F19" s="53" t="s">
-        <v>91</v>
-      </c>
-      <c r="G19" s="47" t="s">
-        <v>92</v>
-      </c>
-      <c r="H19" s="54" t="s">
-        <v>93</v>
-      </c>
-      <c r="I19" s="58"/>
-      <c r="J19" s="60"/>
-      <c r="K19" s="58"/>
-    </row>
-    <row r="20" spans="1:11" ht="102" customHeight="1">
-      <c r="A20" s="51" t="s">
-        <v>94</v>
-      </c>
-      <c r="B20" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="C20" s="40" t="s">
-        <v>95</v>
-      </c>
-      <c r="D20" s="57" t="s">
-        <v>22</v>
-      </c>
-      <c r="E20" s="40" t="s">
-        <v>96</v>
-      </c>
-      <c r="F20" s="53" t="s">
-        <v>24</v>
-      </c>
-      <c r="G20" s="47" t="s">
-        <v>97</v>
-      </c>
-      <c r="H20" s="59"/>
-      <c r="I20" s="58"/>
-      <c r="J20" s="60"/>
-      <c r="K20" s="58"/>
-    </row>
-    <row r="21" spans="1:11" ht="78" customHeight="1">
-      <c r="A21" s="51" t="s">
-        <v>98</v>
-      </c>
-      <c r="B21" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="C21" s="40" t="s">
-        <v>99</v>
-      </c>
-      <c r="D21" s="57" t="s">
-        <v>22</v>
-      </c>
-      <c r="E21" s="40" t="s">
-        <v>100</v>
-      </c>
-      <c r="F21" s="53" t="s">
-        <v>24</v>
-      </c>
-      <c r="G21" s="47" t="s">
-        <v>101</v>
-      </c>
-      <c r="H21" s="59"/>
-      <c r="I21" s="58"/>
-      <c r="J21" s="60"/>
-      <c r="K21" s="58"/>
-    </row>
-    <row r="22" spans="1:11" ht="69" customHeight="1">
-      <c r="A22" s="51" t="s">
-        <v>102</v>
-      </c>
-      <c r="B22" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="C22" s="40" t="s">
-        <v>103</v>
-      </c>
-      <c r="D22" s="57" t="s">
-        <v>22</v>
-      </c>
-      <c r="E22" s="40" t="s">
-        <v>104</v>
-      </c>
-      <c r="F22" s="53" t="s">
-        <v>24</v>
-      </c>
-      <c r="G22" s="47" t="s">
-        <v>105</v>
-      </c>
-      <c r="H22" s="59"/>
-      <c r="I22" s="58"/>
-      <c r="J22" s="60"/>
-      <c r="K22" s="58"/>
-    </row>
-    <row r="23" spans="1:11" ht="124.5" customHeight="1">
-      <c r="A23" s="51" t="s">
-        <v>106</v>
-      </c>
-      <c r="B23" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="C23" s="40" t="s">
-        <v>107</v>
-      </c>
-      <c r="D23" s="57" t="s">
-        <v>22</v>
-      </c>
-      <c r="E23" s="40" t="s">
-        <v>108</v>
-      </c>
-      <c r="F23" s="53" t="s">
-        <v>24</v>
-      </c>
-      <c r="G23" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="H23" s="59"/>
-      <c r="I23" s="58"/>
-      <c r="J23" s="60"/>
-      <c r="K23" s="58"/>
-    </row>
-    <row r="24" spans="1:11" ht="107.25">
-      <c r="A24" s="51" t="s">
-        <v>110</v>
-      </c>
-      <c r="B24" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="C24" s="40" t="s">
-        <v>111</v>
-      </c>
-      <c r="D24" s="57" t="s">
-        <v>22</v>
-      </c>
-      <c r="E24" s="40" t="s">
-        <v>112</v>
-      </c>
-      <c r="F24" s="53" t="s">
-        <v>24</v>
-      </c>
-      <c r="G24" s="47" t="s">
-        <v>113</v>
-      </c>
-      <c r="H24" s="59" t="s">
-        <v>114</v>
-      </c>
-      <c r="I24" s="58"/>
-      <c r="J24" s="60"/>
-      <c r="K24" s="58"/>
-    </row>
-    <row r="25" spans="1:11" ht="91.5">
-      <c r="A25" s="51" t="s">
-        <v>115</v>
-      </c>
-      <c r="B25" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="C25" s="40" t="s">
-        <v>111</v>
-      </c>
-      <c r="D25" s="57" t="s">
-        <v>22</v>
-      </c>
-      <c r="E25" s="40" t="s">
-        <v>116</v>
-      </c>
-      <c r="F25" s="53" t="s">
-        <v>24</v>
-      </c>
-      <c r="G25" s="47" t="s">
-        <v>117</v>
-      </c>
-      <c r="H25" s="59"/>
-      <c r="I25" s="58"/>
-      <c r="J25" s="60"/>
-      <c r="K25" s="58"/>
-    </row>
-    <row r="26" spans="1:11" ht="74.25" customHeight="1">
-      <c r="A26" s="51" t="s">
-        <v>118</v>
-      </c>
-      <c r="B26" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="C26" s="40" t="s">
-        <v>119</v>
-      </c>
-      <c r="D26" s="57" t="s">
-        <v>22</v>
-      </c>
-      <c r="E26" s="40" t="s">
-        <v>120</v>
-      </c>
-      <c r="F26" s="53" t="s">
-        <v>24</v>
-      </c>
-      <c r="G26" s="47" t="s">
-        <v>121</v>
-      </c>
-      <c r="H26" s="59"/>
-      <c r="I26" s="58"/>
-      <c r="J26" s="60"/>
-      <c r="K26" s="58"/>
-    </row>
-    <row r="27" spans="1:11" s="6" customFormat="1" ht="83.25" customHeight="1">
-      <c r="A27" s="51" t="s">
-        <v>118</v>
-      </c>
-      <c r="B27" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="C27" s="69" t="s">
+      <c r="E27" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="D27" s="57" t="s">
-        <v>22</v>
-      </c>
-      <c r="E27" s="40" t="s">
-        <v>120</v>
-      </c>
-      <c r="F27" s="48" t="s">
-        <v>24</v>
-      </c>
-      <c r="G27" s="46" t="s">
-        <v>123</v>
-      </c>
-      <c r="H27" s="62"/>
-      <c r="I27" s="63"/>
-      <c r="J27" s="64"/>
-      <c r="K27" s="63"/>
+      <c r="F27" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="G27" s="45" t="s">
+        <v>125</v>
+      </c>
+      <c r="H27" s="61"/>
+      <c r="I27" s="62"/>
+      <c r="J27" s="63"/>
+      <c r="K27" s="62"/>
     </row>
     <row r="28" spans="1:11" ht="51.75" customHeight="1">
-      <c r="C28" s="66"/>
-      <c r="D28" s="66"/>
+      <c r="C28" s="64"/>
+      <c r="D28" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3045,7 +3115,7 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
@@ -3053,7 +3123,7 @@
     <col min="1" max="1" width="19" style="20" customWidth="1"/>
     <col min="2" max="2" width="17.140625" style="20" customWidth="1"/>
     <col min="3" max="3" width="27.42578125" style="21" customWidth="1"/>
-    <col min="4" max="4" width="31" style="35" customWidth="1"/>
+    <col min="4" max="4" width="31" style="34" customWidth="1"/>
     <col min="5" max="5" width="49" style="22" customWidth="1"/>
     <col min="6" max="6" width="23.7109375" style="10" customWidth="1"/>
     <col min="7" max="7" width="43.5703125" style="22" customWidth="1"/>
@@ -3064,77 +3134,77 @@
     <col min="12" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="73" customFormat="1" ht="15.75">
+    <row r="1" spans="1:11" s="71" customFormat="1" ht="15.75">
       <c r="A1" s="9" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="C1" s="72" t="s">
-        <v>10</v>
+        <v>126</v>
+      </c>
+      <c r="C1" s="70" t="s">
+        <v>12</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="K1" s="9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" s="33" customFormat="1" ht="18.75">
-      <c r="A2" s="29" t="s">
-        <v>125</v>
-      </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="32" customFormat="1" ht="18.75">
+      <c r="A2" s="93" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" s="93"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
     </row>
     <row r="3" spans="1:11" ht="110.25" customHeight="1">
       <c r="A3" s="11" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
@@ -3143,25 +3213,25 @@
     </row>
     <row r="4" spans="1:11" ht="117.75" customHeight="1">
       <c r="A4" s="11" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="H4" s="17"/>
       <c r="I4" s="17"/>
@@ -3174,22 +3244,22 @@
         <v>TC_LF_003</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E5" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="G5" s="13" t="s">
         <v>140</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="G5" s="13" t="s">
-        <v>138</v>
       </c>
       <c r="H5" s="17"/>
       <c r="I5" s="17"/>
@@ -3202,22 +3272,22 @@
         <v>TC_LF_004</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="H6" s="17"/>
       <c r="I6" s="17"/>
@@ -3230,20 +3300,20 @@
         <v>TC_LF_005</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="F7" s="16"/>
       <c r="G7" s="13" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="H7" s="17"/>
       <c r="I7" s="17"/>
@@ -3256,20 +3326,20 @@
         <v>TC_LF_006</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="F8" s="16"/>
       <c r="G8" s="13" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="H8" s="17"/>
       <c r="I8" s="17"/>
@@ -3282,20 +3352,20 @@
         <v>TC_LF_007</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="F9" s="16"/>
       <c r="G9" s="13" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="H9" s="17"/>
       <c r="I9" s="17"/>
@@ -3308,22 +3378,22 @@
         <v>TC_LF_008</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="C10" s="36" t="s">
-        <v>153</v>
+        <v>129</v>
+      </c>
+      <c r="C10" s="35" t="s">
+        <v>155</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="H10" s="17"/>
       <c r="I10" s="17"/>
@@ -3336,20 +3406,20 @@
         <v>TC_LF_009</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F11" s="16"/>
       <c r="G11" s="13" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="H11" s="17"/>
       <c r="I11" s="17"/>
@@ -3362,26 +3432,26 @@
         <v>TC_LF_010</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="C12" s="37" t="s">
-        <v>159</v>
+        <v>129</v>
+      </c>
+      <c r="C12" s="36" t="s">
+        <v>161</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="H12" s="13"/>
       <c r="I12" s="13"/>
-      <c r="J12" s="38"/>
+      <c r="J12" s="37"/>
       <c r="K12" s="13"/>
     </row>
     <row r="13" spans="1:11" ht="122.25">
@@ -3390,26 +3460,26 @@
         <v>TC_LF_011</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="C13" s="37" t="s">
-        <v>162</v>
+        <v>129</v>
+      </c>
+      <c r="C13" s="36" t="s">
+        <v>164</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="H13" s="13"/>
       <c r="I13" s="13"/>
-      <c r="J13" s="38"/>
+      <c r="J13" s="37"/>
       <c r="K13" s="13"/>
     </row>
     <row r="14" spans="1:11" ht="91.5">
@@ -3418,24 +3488,24 @@
         <v>TC_LF_012</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="F14" s="12"/>
       <c r="G14" s="12" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="H14" s="12"/>
       <c r="I14" s="12"/>
-      <c r="J14" s="39"/>
+      <c r="J14" s="38"/>
       <c r="K14" s="12"/>
     </row>
     <row r="15" spans="1:11" ht="128.25" customHeight="1">
@@ -3444,20 +3514,20 @@
         <v>TC_LF_013</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="C15" s="40" t="s">
-        <v>95</v>
+        <v>129</v>
+      </c>
+      <c r="C15" s="39" t="s">
+        <v>97</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="E15" s="41" t="s">
-        <v>168</v>
+        <v>137</v>
+      </c>
+      <c r="E15" s="40" t="s">
+        <v>170</v>
       </c>
       <c r="F15" s="16"/>
       <c r="G15" s="13" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="H15" s="17"/>
       <c r="I15" s="17"/>
@@ -3470,26 +3540,26 @@
         <v>TC_LF_014</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="C16" s="37" t="s">
-        <v>170</v>
+        <v>129</v>
+      </c>
+      <c r="C16" s="36" t="s">
+        <v>172</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G16" s="13" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="H16" s="13"/>
       <c r="I16" s="13"/>
-      <c r="J16" s="38"/>
+      <c r="J16" s="37"/>
       <c r="K16" s="13"/>
     </row>
     <row r="17" spans="1:11" ht="99" customHeight="1">
@@ -3498,26 +3568,26 @@
         <v>TC_LF_015</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="C17" s="37" t="s">
-        <v>173</v>
+        <v>129</v>
+      </c>
+      <c r="C17" s="36" t="s">
+        <v>175</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="H17" s="13"/>
       <c r="I17" s="13"/>
-      <c r="J17" s="38"/>
+      <c r="J17" s="37"/>
       <c r="K17" s="13"/>
     </row>
     <row r="18" spans="1:11" ht="138.75" customHeight="1">
@@ -3526,27 +3596,27 @@
         <v>TC_LF_016</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="E18" s="42" t="s">
-        <v>177</v>
+        <v>137</v>
+      </c>
+      <c r="E18" s="41" t="s">
+        <v>179</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="G18" s="42" t="s">
-        <v>178</v>
-      </c>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="43"/>
-      <c r="K18" s="42"/>
+        <v>26</v>
+      </c>
+      <c r="G18" s="41" t="s">
+        <v>180</v>
+      </c>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="42"/>
+      <c r="K18" s="41"/>
     </row>
     <row r="19" spans="1:11" ht="105.75" customHeight="1">
       <c r="A19" s="14" t="str">
@@ -3554,22 +3624,22 @@
         <v>TC_LF_017</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G19" s="19" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="H19" s="17"/>
       <c r="I19" s="17"/>
@@ -3582,22 +3652,22 @@
         <v>TC_LF_018</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G20" s="13" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="H20" s="17"/>
       <c r="I20" s="17"/>
@@ -3610,22 +3680,22 @@
         <v>TC_LF_019</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G21" s="13" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="H21" s="17"/>
       <c r="I21" s="17"/>
@@ -3693,4 +3763,510 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A75320F2-3481-43C3-BBE2-CA0639B632EF}">
+  <dimension ref="A1:K9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="15.7109375" style="79"/>
+    <col min="3" max="3" width="24.5703125" style="83" customWidth="1"/>
+    <col min="4" max="4" width="32.28515625" style="81" customWidth="1"/>
+    <col min="5" max="5" width="38.7109375" style="88" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" style="82" customWidth="1"/>
+    <col min="7" max="7" width="35.42578125" style="88" customWidth="1"/>
+    <col min="8" max="8" width="29.85546875" style="88" customWidth="1"/>
+    <col min="9" max="16384" width="15.7109375" style="79"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="74" customFormat="1" ht="15" customHeight="1">
+      <c r="A1" s="73" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="73" t="s">
+        <v>126</v>
+      </c>
+      <c r="C1" s="73" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="84" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="80" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="85" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="80" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="80" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="73" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="73" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="73" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="78" customFormat="1">
+      <c r="A2" s="94" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="94"/>
+      <c r="C2" s="87"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="76"/>
+      <c r="J2" s="76"/>
+      <c r="K2" s="76"/>
+    </row>
+    <row r="3" spans="1:11" ht="57" customHeight="1">
+      <c r="A3" s="77" t="s">
+        <v>190</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="83" t="s">
+        <v>191</v>
+      </c>
+      <c r="D3" s="86" t="s">
+        <v>192</v>
+      </c>
+      <c r="E3" s="88" t="s">
+        <v>193</v>
+      </c>
+      <c r="F3" s="82" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="88" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="76.5">
+      <c r="A4" s="77" t="s">
+        <v>195</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="83" t="s">
+        <v>196</v>
+      </c>
+      <c r="D4" s="86" t="s">
+        <v>192</v>
+      </c>
+      <c r="E4" s="88" t="s">
+        <v>197</v>
+      </c>
+      <c r="F4" s="82" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="88" t="s">
+        <v>198</v>
+      </c>
+      <c r="H4" s="88" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="45.75">
+      <c r="A5" s="77" t="s">
+        <v>200</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="83" t="s">
+        <v>201</v>
+      </c>
+      <c r="D5" s="86" t="s">
+        <v>137</v>
+      </c>
+      <c r="E5" s="88" t="s">
+        <v>202</v>
+      </c>
+      <c r="F5" s="82" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="88" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="107.25">
+      <c r="A6" s="77" t="s">
+        <v>204</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="83" t="s">
+        <v>205</v>
+      </c>
+      <c r="D6" s="86" t="s">
+        <v>206</v>
+      </c>
+      <c r="E6" s="88" t="s">
+        <v>207</v>
+      </c>
+      <c r="F6" s="82" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="88" t="s">
+        <v>208</v>
+      </c>
+      <c r="H6" s="88" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="107.25" customHeight="1">
+      <c r="A7" s="77" t="s">
+        <v>210</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="83" t="s">
+        <v>211</v>
+      </c>
+      <c r="D7" s="86" t="s">
+        <v>137</v>
+      </c>
+      <c r="E7" s="88" t="s">
+        <v>212</v>
+      </c>
+      <c r="F7" s="82" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="88" t="s">
+        <v>213</v>
+      </c>
+      <c r="H7" s="88" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="76.5">
+      <c r="A8" s="77" t="s">
+        <v>215</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="83" t="s">
+        <v>216</v>
+      </c>
+      <c r="D8" s="86" t="s">
+        <v>137</v>
+      </c>
+      <c r="E8" s="88" t="s">
+        <v>217</v>
+      </c>
+      <c r="F8" s="82" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="88" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="61.5">
+      <c r="A9" s="77" t="s">
+        <v>219</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="83" t="s">
+        <v>220</v>
+      </c>
+      <c r="D9" s="86" t="s">
+        <v>137</v>
+      </c>
+      <c r="E9" s="88" t="s">
+        <v>193</v>
+      </c>
+      <c r="F9" s="82" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="88" t="s">
+        <v>221</v>
+      </c>
+      <c r="H9" s="88" t="s">
+        <v>222</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:B2"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A2" location="'Test Scenarios'!A10" display="&lt;&lt; Test Scenarios" xr:uid="{151E21E0-4609-421E-8344-6890EA1E5ED1}"/>
+    <hyperlink ref="B2" location="'Test Scenarios'!A10" display="&lt;&lt; Test Scenarios" xr:uid="{98089D30-9841-4241-9256-01B88778A559}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E84AD250-2B76-4ED5-91E2-B1D4742B666B}">
+  <dimension ref="A1:K33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" style="97" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" style="97" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" style="83" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" style="97" customWidth="1"/>
+    <col min="5" max="5" width="39.5703125" style="88" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" style="97" customWidth="1"/>
+    <col min="7" max="7" width="37.7109375" style="97" customWidth="1"/>
+    <col min="8" max="8" width="35.42578125" style="97" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" style="97" customWidth="1"/>
+    <col min="10" max="10" width="13" style="97" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" style="97" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="97"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="74" customFormat="1">
+      <c r="A1" s="95" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="95" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="95" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="95" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="100" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="95" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="95" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="95" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="95" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="95" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="95" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="96" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="96"/>
+    </row>
+    <row r="3" spans="1:11" ht="75.75" customHeight="1">
+      <c r="A3" s="98" t="s">
+        <v>223</v>
+      </c>
+      <c r="B3" s="91" t="s">
+        <v>224</v>
+      </c>
+      <c r="C3" s="99" t="s">
+        <v>225</v>
+      </c>
+      <c r="D3" s="99" t="s">
+        <v>137</v>
+      </c>
+      <c r="E3" s="101" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="98" t="s">
+        <v>227</v>
+      </c>
+      <c r="B4" s="90"/>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="98" t="s">
+        <v>228</v>
+      </c>
+      <c r="B5" s="90"/>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="98" t="s">
+        <v>229</v>
+      </c>
+      <c r="B6" s="90"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="98" t="s">
+        <v>230</v>
+      </c>
+      <c r="B7" s="90"/>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="98" t="s">
+        <v>231</v>
+      </c>
+      <c r="B8" s="90"/>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="98" t="s">
+        <v>232</v>
+      </c>
+      <c r="B9" s="90"/>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="98" t="s">
+        <v>233</v>
+      </c>
+      <c r="B10" s="90"/>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="98" t="s">
+        <v>234</v>
+      </c>
+      <c r="B11" s="90"/>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="98" t="s">
+        <v>235</v>
+      </c>
+      <c r="B12" s="90"/>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="98" t="s">
+        <v>236</v>
+      </c>
+      <c r="B13" s="90"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="98" t="s">
+        <v>237</v>
+      </c>
+      <c r="B14" s="90"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="98"/>
+      <c r="B15" s="90"/>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="98"/>
+      <c r="B16" s="90"/>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="98"/>
+      <c r="B17" s="90"/>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="98"/>
+      <c r="B18" s="90"/>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="98"/>
+      <c r="B19" s="90"/>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="98"/>
+      <c r="B20" s="90"/>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="98"/>
+      <c r="B21" s="90"/>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="98"/>
+      <c r="B22" s="90"/>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="98"/>
+      <c r="B23" s="90"/>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="98"/>
+      <c r="B24" s="90"/>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="98"/>
+      <c r="B25" s="90"/>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="98"/>
+      <c r="B26" s="90"/>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="98"/>
+      <c r="B27" s="90"/>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="98"/>
+      <c r="B28" s="90"/>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="98"/>
+      <c r="B29" s="90"/>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="98"/>
+      <c r="B30" s="90"/>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="98"/>
+      <c r="B31" s="90"/>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="98"/>
+      <c r="B32" s="90"/>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="98"/>
+      <c r="B33" s="90"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:B2"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A2" location="'Test Scenarios'!A10" display="&lt;&lt; Test Scenarios" xr:uid="{15A4A597-E448-4664-8F3B-A510F0A9D0F0}"/>
+    <hyperlink ref="B2" location="'Test Scenarios'!A10" display="&lt;&lt; Test Scenarios" xr:uid="{9E60975B-84D9-44FC-B3AB-C6D6873048C2}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C762F33A-E1B7-4052-AF92-AAE1CE47BB02}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>